<commit_message>
Ajout de multiple falls et modify excel
</commit_message>
<xml_diff>
--- a/Experiences/Experiences.xlsx
+++ b/Experiences/Experiences.xlsx
@@ -18,8 +18,93 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+    <author>Clémence Briosne Fréjaville</author>
+  </authors>
+  <commentList>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Clémence Briosne Fréjaville:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -118,13 +203,37 @@
   </si>
   <si>
     <t>A dose of 20*0.10044*df=2.0088pC is enough to pierce through the membrane with dots. Concerning lines, a dose of higherDF*( 20*3000μC/cm=60000μC/cm) is not enough to pierce through the membrane.</t>
+  </si>
+  <si>
+    <t>Dots piercing</t>
+  </si>
+  <si>
+    <t>Area piercing (pC)</t>
+  </si>
+  <si>
+    <t>Area/Line Step size</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Line piercing: yes/no</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>dose factor</t>
+  </si>
+  <si>
+    <t>total current</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -150,6 +259,54 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,18 +325,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,16 +695,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="15" width="17.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="3"/>
+    <col min="17" max="25" width="9.5" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:25" ht="54">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,104 +749,153 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="18">
-      <c r="A2" s="3">
+    <row r="2" spans="1:25" ht="30">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="112">
+      <c r="A3" s="4">
         <v>42545</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="1">
         <v>20</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I3" s="1">
         <v>6.8120000000000003</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J3" s="5">
         <v>0.10044</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K3" s="1">
         <v>1000</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L3" s="1">
         <v>1000</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="1" t="s">
+      <c r="M3" s="1">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="Q3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="S3" s="3">
+        <f>F3*H3*J3*R3</f>
+        <v>2.8123199999999997</v>
+      </c>
+      <c r="V3" s="3">
+        <f>F3*H3*K3*M3*U3</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="3">
+        <f>F3*H3*L3*M3*X3</f>
+        <v>640</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="16">
-      <c r="A3" s="5">
+    <row r="4" spans="1:25" ht="42">
+      <c r="A4" s="6">
         <v>42548</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2.0087999999999999</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2">
-        <v>20000</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="16">
-      <c r="A4" s="5">
-        <v>42549</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -664,19 +907,19 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>24</v>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>0.878</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="J4" s="2">
         <v>2.0087999999999999</v>
@@ -685,16 +928,29 @@
       <c r="L4" s="2">
         <v>20000</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>26</v>
+      <c r="M4" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="S4" s="3">
+        <f t="shared" ref="S4:S9" si="0">F4*H4*J4*R4</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <f t="shared" ref="V4:V9" si="1">F4*H4*K4*M4*U4</f>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <f t="shared" ref="Y4:Y9" si="2">F4*H4*L4*M4*X4</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16">
-      <c r="A5" s="5">
+    <row r="5" spans="1:25" ht="140">
+      <c r="A5" s="6">
         <v>42549</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -712,30 +968,47 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>0.26</v>
+        <v>0.878</v>
       </c>
       <c r="J5" s="2">
-        <v>0.10044</v>
+        <v>2.0087999999999999</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="2"/>
+        <v>20000</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="16">
-      <c r="A6" s="5">
+    <row r="6" spans="1:25" ht="32">
+      <c r="A6" s="6">
         <v>42549</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -748,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -757,27 +1030,42 @@
         <v>27</v>
       </c>
       <c r="H6" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I6" s="2">
-        <v>0.77100000000000002</v>
+        <v>0.26</v>
       </c>
       <c r="J6" s="2">
-        <v>2.0087999999999999</v>
-      </c>
-      <c r="K6" s="2">
-        <v>20000</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="2"/>
+        <v>0.10044</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="S6" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="16">
-      <c r="A7" s="5">
-        <v>42551</v>
+    <row r="7" spans="1:25" ht="336">
+      <c r="A7" s="6">
+        <v>42549</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -789,33 +1077,50 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H7" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>6.95</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="J7" s="2">
-        <v>0.10044</v>
+        <v>2.0087999999999999</v>
       </c>
       <c r="K7" s="2">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="2"/>
+      <c r="M7" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="S7" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" ht="16">
-      <c r="A8" s="5">
+    <row r="8" spans="1:25" ht="32">
+      <c r="A8" s="6">
         <v>42551</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -841,17 +1146,94 @@
         <v>6.95</v>
       </c>
       <c r="J8" s="2">
+        <v>0.10044</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="S8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="32">
+      <c r="A9" s="6">
+        <v>42551</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2">
+        <v>6.95</v>
+      </c>
+      <c r="J9" s="2">
         <v>0.8</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K9" s="2">
         <v>3000</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="11"/>
+      <c r="S9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>